<commit_message>
Udpated Status Column as null
Udpated Status Column as null
</commit_message>
<xml_diff>
--- a/MavenCucumerSampleTest/TestData/TestData_Guru99Bank.xlsx
+++ b/MavenCucumerSampleTest/TestData/TestData_Guru99Bank.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="12645" windowWidth="22260" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomer" r:id="rId1" sheetId="1"/>
-    <sheet name="Tools_QA_Practice" r:id="rId2" sheetId="3"/>
+    <sheet name="AddCustomer" sheetId="1" r:id="rId1"/>
+    <sheet name="Tools_QA_Practice" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Iteration</t>
   </si>
@@ -149,19 +149,12 @@
   </si>
   <si>
     <t>47138</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Success</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -197,21 +190,21 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -228,10 +221,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -266,7 +259,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -301,7 +294,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -395,21 +388,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -426,7 +419,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -478,15 +471,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
@@ -494,7 +487,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -575,16 +568,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="J2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45504894-FA84-4B2E-94D3-624EEB35D524}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45504894-FA84-4B2E-94D3-624EEB35D524}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
@@ -592,7 +585,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -630,7 +623,7 @@
         <v>39</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -664,11 +657,9 @@
       <c r="K2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L2" t="s">
-        <v>44</v>
-      </c>
+      <c r="L2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Script to handle Upload & DownLoad Functionalities
Updated Script to handle Upload & DownLoad Functionalities
</commit_message>
<xml_diff>
--- a/MavenCucumerSampleTest/TestData/TestData_Guru99Bank.xlsx
+++ b/MavenCucumerSampleTest/TestData/TestData_Guru99Bank.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="1" windowHeight="12645" windowWidth="22260" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomer" sheetId="1" r:id="rId1"/>
-    <sheet name="Tools_QA_Practice" sheetId="3" r:id="rId2"/>
+    <sheet name="AddCustomer" r:id="rId1" sheetId="1"/>
+    <sheet name="Tools_QA_Practice" r:id="rId2" sheetId="3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
   <si>
     <t>Iteration</t>
   </si>
@@ -149,12 +149,19 @@
   </si>
   <si>
     <t>47138</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Success</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -190,21 +197,21 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -221,10 +228,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -259,7 +266,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -294,7 +301,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -388,21 +395,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -419,7 +426,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -471,15 +478,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
@@ -487,7 +494,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -568,16 +575,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink r:id="rId1" ref="J2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45504894-FA84-4B2E-94D3-624EEB35D524}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45504894-FA84-4B2E-94D3-624EEB35D524}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
@@ -585,7 +592,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,7 +630,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -657,9 +664,11 @@
       <c r="K2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L2"/>
+      <c r="L2" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Test Data Sheet With Continent Value
Updated Test Data Sheet With Continent Value
</commit_message>
<xml_diff>
--- a/MavenCucumerSampleTest/TestData/TestData_Guru99Bank.xlsx
+++ b/MavenCucumerSampleTest/TestData/TestData_Guru99Bank.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="12645" windowWidth="22260" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomer" r:id="rId1" sheetId="1"/>
-    <sheet name="Tools_QA_Practice" r:id="rId2" sheetId="3"/>
+    <sheet name="AddCustomer" sheetId="1" r:id="rId1"/>
+    <sheet name="Tools_QA_Practice" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Iteration</t>
   </si>
@@ -136,9 +136,6 @@
     <t>Selenium IDE</t>
   </si>
   <si>
-    <t>North America</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -151,17 +148,13 @@
     <t>47138</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>Success</t>
+    <t>South America</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -197,21 +190,21 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -228,10 +221,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -266,7 +259,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -301,7 +294,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -395,21 +388,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -426,7 +419,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -478,15 +471,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
@@ -494,7 +487,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -564,35 +557,35 @@
         <v>18</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="J2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45504894-FA84-4B2E-94D3-624EEB35D524}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45504894-FA84-4B2E-94D3-624EEB35D524}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,10 +620,10 @@
         <v>30</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -644,7 +637,7 @@
         <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>34</v>
@@ -659,16 +652,14 @@
         <v>37</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L2" t="s">
-        <v>44</v>
-      </c>
+      <c r="L2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>